<commit_message>
Feat: report with logit classifier
</commit_message>
<xml_diff>
--- a/fangorn/baselines/baseline_classifier.xlsx
+++ b/fangorn/baselines/baseline_classifier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
   <si>
     <t>dataset</t>
   </si>
@@ -73,6 +73,9 @@
     <t>rf_baseline</t>
   </si>
   <si>
+    <t>logit_baseline</t>
+  </si>
+  <si>
     <t>(3467, 1636)</t>
   </si>
   <si>
@@ -88,49 +91,64 @@
     <t>(3279, 20)</t>
   </si>
   <si>
-    <t>1.117</t>
-  </si>
-  <si>
-    <t>8.643</t>
-  </si>
-  <si>
-    <t>1.895</t>
+    <t>1.132</t>
+  </si>
+  <si>
+    <t>8.614</t>
+  </si>
+  <si>
+    <t>1.871</t>
+  </si>
+  <si>
+    <t>132.973</t>
   </si>
   <si>
     <t>0.038</t>
   </si>
   <si>
-    <t>0.207</t>
-  </si>
-  <si>
-    <t>0.263</t>
-  </si>
-  <si>
-    <t>0.335</t>
-  </si>
-  <si>
-    <t>1.787</t>
+    <t>0.233</t>
+  </si>
+  <si>
+    <t>0.253</t>
+  </si>
+  <si>
+    <t>0.024</t>
+  </si>
+  <si>
+    <t>0.346</t>
+  </si>
+  <si>
+    <t>1.735</t>
   </si>
   <si>
     <t>1.393</t>
   </si>
   <si>
-    <t>0.106</t>
-  </si>
-  <si>
-    <t>0.758</t>
-  </si>
-  <si>
-    <t>0.539</t>
-  </si>
-  <si>
-    <t>0.028</t>
-  </si>
-  <si>
-    <t>0.179</t>
-  </si>
-  <si>
-    <t>0.393</t>
+    <t>3.765</t>
+  </si>
+  <si>
+    <t>0.097</t>
+  </si>
+  <si>
+    <t>0.781</t>
+  </si>
+  <si>
+    <t>0.532</t>
+  </si>
+  <si>
+    <t>0.653</t>
+  </si>
+  <si>
+    <t>0.034</t>
+  </si>
+  <si>
+    <t>0.184</t>
+  </si>
+  <si>
+    <t>0.397</t>
+  </si>
+  <si>
+    <t>0.085</t>
   </si>
   <si>
     <t>(1084, 1636)</t>
@@ -148,37 +166,43 @@
     <t>(1025, 20)</t>
   </si>
   <si>
-    <t>0.030</t>
-  </si>
-  <si>
-    <t>0.024</t>
+    <t>0.045</t>
+  </si>
+  <si>
+    <t>0.026</t>
   </si>
   <si>
     <t>0.023</t>
   </si>
   <si>
-    <t>0.005</t>
+    <t>0.009</t>
+  </si>
+  <si>
+    <t>0.004</t>
+  </si>
+  <si>
+    <t>0.007</t>
+  </si>
+  <si>
+    <t>0.015</t>
+  </si>
+  <si>
+    <t>0.003</t>
+  </si>
+  <si>
+    <t>0.013</t>
+  </si>
+  <si>
+    <t>0.010</t>
+  </si>
+  <si>
+    <t>0.020</t>
+  </si>
+  <si>
+    <t>0.017</t>
   </si>
   <si>
     <t>0.006</t>
-  </si>
-  <si>
-    <t>0.016</t>
-  </si>
-  <si>
-    <t>0.008</t>
-  </si>
-  <si>
-    <t>0.009</t>
-  </si>
-  <si>
-    <t>0.019</t>
-  </si>
-  <si>
-    <t>0.015</t>
-  </si>
-  <si>
-    <t>0.003</t>
   </si>
 </sst>
 </file>
@@ -536,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -585,16 +609,16 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G2">
         <v>0.7306273062730627</v>
@@ -620,16 +644,16 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G3">
         <v>0.7416974169741697</v>
@@ -655,16 +679,16 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G4">
         <v>0.7214022140221402</v>
@@ -684,37 +708,37 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="G5">
-        <v>0.8107202680067002</v>
+        <v>0.6171586715867159</v>
       </c>
       <c r="H5">
-        <v>0.830954954954955</v>
+        <v>0.6170220733417759</v>
       </c>
       <c r="I5">
-        <v>0.8092602985744752</v>
+        <v>0.6171916283414529</v>
       </c>
       <c r="J5">
-        <v>0.8330871491875923</v>
+        <v>0.6081208687440982</v>
       </c>
       <c r="K5">
-        <v>0.8675103827590077</v>
+        <v>0.6671382741892045</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -722,34 +746,34 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G6">
-        <v>0.8040201005025126</v>
+        <v>0.8107202680067002</v>
       </c>
       <c r="H6">
-        <v>0.814968487394958</v>
+        <v>0.830954954954955</v>
       </c>
       <c r="I6">
-        <v>0.8029127848243349</v>
+        <v>0.8092602985744752</v>
       </c>
       <c r="J6">
-        <v>0.8224582701062215</v>
+        <v>0.8330871491875923</v>
       </c>
       <c r="K6">
-        <v>0.8710854192389719</v>
+        <v>0.8675103827590077</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -757,104 +781,104 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G7">
-        <v>0.7839195979899497</v>
+        <v>0.8040201005025126</v>
       </c>
       <c r="H7">
-        <v>0.8407516100105976</v>
+        <v>0.814968487394958</v>
       </c>
       <c r="I7">
-        <v>0.7815130766640477</v>
+        <v>0.8029127848243349</v>
       </c>
       <c r="J7">
-        <v>0.8220689655172414</v>
+        <v>0.8224582701062215</v>
       </c>
       <c r="K7">
-        <v>0.8644404534740149</v>
+        <v>0.8710854192389719</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G8">
-        <v>0.7557840616966581</v>
+        <v>0.7839195979899497</v>
       </c>
       <c r="H8">
-        <v>0.7596903129462936</v>
+        <v>0.8407516100105976</v>
       </c>
       <c r="I8">
-        <v>0.7577429334337101</v>
+        <v>0.7815130766640477</v>
       </c>
       <c r="J8">
-        <v>0.7484554280670784</v>
+        <v>0.8220689655172414</v>
       </c>
       <c r="K8">
-        <v>0.8453104231117593</v>
+        <v>0.8644404534740149</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="G9">
-        <v>0.7660668380462725</v>
+        <v>0.7772194304857621</v>
       </c>
       <c r="H9">
-        <v>0.7682151913663974</v>
+        <v>0.7850045167118338</v>
       </c>
       <c r="I9">
-        <v>0.7674958535753356</v>
+        <v>0.7762262880233471</v>
       </c>
       <c r="J9">
-        <v>0.7628149435273676</v>
+        <v>0.7963246554364471</v>
       </c>
       <c r="K9">
-        <v>0.8611212402808982</v>
+        <v>0.8537770793579526</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -862,144 +886,144 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="G10">
-        <v>0.7052270779777207</v>
+        <v>0.7557840616966581</v>
       </c>
       <c r="H10">
-        <v>0.7320433316287229</v>
+        <v>0.7596903129462936</v>
       </c>
       <c r="I10">
-        <v>0.7108309905543858</v>
+        <v>0.7577429334337101</v>
       </c>
       <c r="J10">
-        <v>0.6594059405940594</v>
+        <v>0.7484554280670784</v>
       </c>
       <c r="K10">
-        <v>0.801292155317422</v>
+        <v>0.8453104231117593</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="G11">
-        <v>0.8264331210191083</v>
+        <v>0.7660668380462725</v>
       </c>
       <c r="H11">
-        <v>0.8263654343526547</v>
+        <v>0.7682151913663974</v>
       </c>
       <c r="I11">
-        <v>0.8270121951219511</v>
+        <v>0.7674958535753356</v>
       </c>
       <c r="J11">
-        <v>0.8304821150855364</v>
+        <v>0.7628149435273676</v>
       </c>
       <c r="K11">
-        <v>0.8932113821138212</v>
+        <v>0.8611212402808982</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G12">
-        <v>0.8152866242038217</v>
+        <v>0.7052270779777207</v>
       </c>
       <c r="H12">
-        <v>0.8152866242038217</v>
+        <v>0.7320433316287229</v>
       </c>
       <c r="I12">
-        <v>0.8159146341463415</v>
+        <v>0.7108309905543858</v>
       </c>
       <c r="J12">
-        <v>0.8193146417445484</v>
+        <v>0.6594059405940594</v>
       </c>
       <c r="K12">
-        <v>0.8934247967479675</v>
+        <v>0.801292155317422</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G13">
-        <v>0.6385350318471338</v>
+        <v>0.7300771208226221</v>
       </c>
       <c r="H13">
-        <v>0.6391011395577744</v>
+        <v>0.7339717741935483</v>
       </c>
       <c r="I13">
-        <v>0.6393089430894309</v>
+        <v>0.7320645077811629</v>
       </c>
       <c r="J13">
-        <v>0.6425196850393701</v>
+        <v>0.7214854111405835</v>
       </c>
       <c r="K13">
-        <v>0.7398069105691056</v>
+        <v>0.7972751226283039</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -1008,33 +1032,33 @@
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G14">
-        <v>0.9395121951219512</v>
+        <v>0.8264331210191083</v>
       </c>
       <c r="H14">
-        <v>0.9422083735022724</v>
+        <v>0.8263654343526547</v>
       </c>
       <c r="I14">
-        <v>0.9402077049629832</v>
+        <v>0.8270121951219511</v>
       </c>
       <c r="J14">
-        <v>0.94106463878327</v>
+        <v>0.8304821150855364</v>
       </c>
       <c r="K14">
-        <v>0.9770397282393444</v>
+        <v>0.8932113821138212</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -1043,33 +1067,33 @@
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="G15">
-        <v>0.9414634146341463</v>
+        <v>0.8152866242038217</v>
       </c>
       <c r="H15">
-        <v>0.9436491072520484</v>
+        <v>0.8152866242038217</v>
       </c>
       <c r="I15">
-        <v>0.9420947201657375</v>
+        <v>0.8159146341463415</v>
       </c>
       <c r="J15">
-        <v>0.9427480916030535</v>
+        <v>0.8193146417445484</v>
       </c>
       <c r="K15">
-        <v>0.9827026780001828</v>
+        <v>0.8934247967479675</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -1078,28 +1102,203 @@
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16">
+        <v>0.6385350318471338</v>
+      </c>
+      <c r="H16">
+        <v>0.6391011395577744</v>
+      </c>
+      <c r="I16">
+        <v>0.6393089430894309</v>
+      </c>
+      <c r="J16">
+        <v>0.6425196850393701</v>
+      </c>
+      <c r="K16">
+        <v>0.7398069105691056</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17">
+        <v>0.5700636942675159</v>
+      </c>
+      <c r="H17">
+        <v>0.5694241390513319</v>
+      </c>
+      <c r="I17">
+        <v>0.5694918699186992</v>
+      </c>
+      <c r="J17">
+        <v>0.5858895705521472</v>
+      </c>
+      <c r="K17">
+        <v>0.598709349593496</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18">
+        <v>0.9395121951219512</v>
+      </c>
+      <c r="H18">
+        <v>0.9422083735022724</v>
+      </c>
+      <c r="I18">
+        <v>0.9402077049629832</v>
+      </c>
+      <c r="J18">
+        <v>0.94106463878327</v>
+      </c>
+      <c r="K18">
+        <v>0.9770397282393444</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19">
+        <v>0.9414634146341463</v>
+      </c>
+      <c r="H19">
+        <v>0.9436491072520484</v>
+      </c>
+      <c r="I19">
+        <v>0.9420947201657375</v>
+      </c>
+      <c r="J19">
+        <v>0.9427480916030535</v>
+      </c>
+      <c r="K19">
+        <v>0.9827026780001828</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
         <v>43</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E20" t="s">
         <v>49</v>
       </c>
-      <c r="G16">
+      <c r="F20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20">
         <v>0.9063414634146342</v>
       </c>
-      <c r="H16">
+      <c r="H20">
         <v>0.9103117588819046</v>
       </c>
-      <c r="I16">
+      <c r="I20">
         <v>0.9071896992962252</v>
       </c>
-      <c r="J16">
+      <c r="J20">
         <v>0.9096045197740114</v>
       </c>
-      <c r="K16">
+      <c r="K20">
         <v>0.9556332449806538</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21">
+        <v>0.9004878048780488</v>
+      </c>
+      <c r="H21">
+        <v>0.9029958377327886</v>
+      </c>
+      <c r="I21">
+        <v>0.9011725771562624</v>
+      </c>
+      <c r="J21">
+        <v>0.903041825095057</v>
+      </c>
+      <c r="K21">
+        <v>0.9598223806477165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>